<commit_message>
version test solvable pour bpl (taille reduite)
</commit_message>
<xml_diff>
--- a/data/input_data_.xlsx
+++ b/data/input_data_.xlsx
@@ -1257,13 +1257,13 @@
         <v>51</v>
       </c>
       <c r="B11" s="21">
-        <v>3200</v>
+        <v>4000</v>
       </c>
       <c r="C11" s="21">
+        <v>4000</v>
+      </c>
+      <c r="D11" s="21">
         <v>3000</v>
-      </c>
-      <c r="D11" s="21">
-        <v>1600</v>
       </c>
       <c r="E11" s="21">
         <v>4000</v>
@@ -2360,46 +2360,46 @@
         <v>93</v>
       </c>
       <c r="B34" s="21">
-        <v>7500</v>
+        <v>4000</v>
       </c>
       <c r="C34" s="21">
-        <v>7500</v>
+        <v>5000</v>
       </c>
       <c r="D34" s="21">
-        <v>7500</v>
+        <v>5000</v>
       </c>
       <c r="E34" s="21">
-        <v>7500</v>
+        <v>5000</v>
       </c>
       <c r="F34" s="21">
-        <v>7500</v>
+        <v>5000</v>
       </c>
       <c r="G34" s="21">
-        <v>7500</v>
+        <v>5000</v>
       </c>
       <c r="H34" s="21">
-        <v>7500</v>
+        <v>5000</v>
       </c>
       <c r="I34" s="21">
-        <v>7500</v>
+        <v>5000</v>
       </c>
       <c r="J34" s="21">
-        <v>7500</v>
+        <v>5000</v>
       </c>
       <c r="K34" s="21">
-        <v>7500</v>
+        <v>5000</v>
       </c>
       <c r="L34" s="21">
-        <v>7500</v>
+        <v>5000</v>
       </c>
       <c r="M34" s="21">
-        <v>7500</v>
+        <v>5000</v>
       </c>
       <c r="N34" s="21">
-        <v>7500</v>
+        <v>5000</v>
       </c>
       <c r="O34" s="21">
-        <v>7500</v>
+        <v>5000</v>
       </c>
       <c r="P34" s="21"/>
       <c r="Q34" s="21"/>

</xml_diff>